<commit_message>
new Spoc added for the new project
</commit_message>
<xml_diff>
--- a/managers_spocs.xlsx
+++ b/managers_spocs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chatadd\slbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86273A0E-7201-4DD7-B0AF-5D05A44849C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4338DC4-59DA-4DB4-954C-A56C5A1E230E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{08CF5315-E4EB-4DC8-95C1-4C362273FE02}"/>
   </bookViews>
@@ -568,7 +568,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>